<commit_message>
update product list manage
</commit_message>
<xml_diff>
--- a/Documents/SE1606_SWP391_OnlineShop_Backlog_W8.xlsx
+++ b/Documents/SE1606_SWP391_OnlineShop_Backlog_W8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RoC" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="183">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -655,13 +655,16 @@
     <t>Add Address User</t>
   </si>
   <si>
-    <t>This is a screen which allows displays the user's address screen, and allows adding more addresses</t>
-  </si>
-  <si>
     <t>Order List</t>
   </si>
   <si>
     <t>Orders Information</t>
+  </si>
+  <si>
+    <t>This is a screen which allows displays the user's address screen, and allows adding more addresses. Allow to choose default address, primary address to be able to contact</t>
+  </si>
+  <si>
+    <t>Manage Products List</t>
   </si>
 </sst>
 </file>
@@ -1832,8 +1835,8 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="8" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,7 +2040,7 @@
         <v>120</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G14" s="39" t="s">
         <v>129</v>
@@ -3004,9 +3007,9 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3202,15 +3205,15 @@
       </c>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>32</v>
+        <v>182</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -3279,7 +3282,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -3573,7 +3576,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="114" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3697,7 +3700,7 @@
         <v>58</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>93</v>
@@ -3872,7 +3875,7 @@
         <v>65</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>11</v>
@@ -4051,9 +4054,9 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>